<commit_message>
First update to github
</commit_message>
<xml_diff>
--- a/Projecto1PR.xlsx
+++ b/Projecto1PR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shared folders\Windows\Shared Documents\Collective\Site\Project1\Projecto1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC8A423-1D6D-4D6A-9222-D40109F1A5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413B038B-7B96-4DBA-A18B-C28BC5BA636E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1320" windowWidth="18300" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4350" yWindow="1635" windowWidth="18300" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>E002</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Proviswion of basics startup artifacts to define project objectives</t>
-  </si>
-  <si>
     <t>I1</t>
   </si>
   <si>
@@ -113,6 +110,24 @@
   </si>
   <si>
     <t>JP</t>
+  </si>
+  <si>
+    <t>App name</t>
+  </si>
+  <si>
+    <t>Suggestion</t>
+  </si>
+  <si>
+    <t>proposals</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Living costs, EXA(employee expenses App), </t>
+  </si>
+  <si>
+    <t>Provision of basics startup artifacts to define project objectives</t>
   </si>
 </sst>
 </file>
@@ -446,13 +461,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE9047A3-F814-4946-A422-C8267F484FE7}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -460,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B760F2-CB8B-4ACA-89C6-D22026A42596}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,13 +527,13 @@
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7E5672-F4AF-469B-9F4A-635B0BEE48C0}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,19 +591,19 @@
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="2">
         <v>44457</v>
@@ -566,19 +611,19 @@
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
       </c>
       <c r="F3" s="2">
         <v>44457</v>
@@ -586,19 +631,19 @@
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
         <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>